<commit_message>
Changes Check and Plan
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="99">
   <si>
     <t>Группа проверок/модуль</t>
   </si>
@@ -211,13 +211,115 @@
   </si>
   <si>
     <t>При нажатии на кнопку "Человечек" кнопка "Log Out" появляется</t>
+  </si>
+  <si>
+    <t>Нефункциональные тесты</t>
+  </si>
+  <si>
+    <t>Зарегистрированный пользователь может пройти аутентификацию и авторизоваться в системе</t>
+  </si>
+  <si>
+    <t>Незарегистрированный пользователь не может пройти аутентификацию и авторизоваться в системе</t>
+  </si>
+  <si>
+    <t>Функциональные тесты</t>
+  </si>
+  <si>
+    <t>В поле Логин спецсимволы ("&amp;" и ";") не вводятся</t>
+  </si>
+  <si>
+    <t>В поле Пароль спецсимволы ("&amp;" и ";") не вводятся</t>
+  </si>
+  <si>
+    <t>Безопасность</t>
+  </si>
+  <si>
+    <t>В поле Категория в разделе редактирования новости спецсимволы ("&amp;" и ";")  не вводятся</t>
+  </si>
+  <si>
+    <t>В поле Заголовок в разделе редактирования новости спецсимволы ("&amp;" и ";")  не вводятся</t>
+  </si>
+  <si>
+    <t>В поле Описание в разделе редактирования новости спецсимволы ("&amp;" и ";")  не вводятся</t>
+  </si>
+  <si>
+    <t>Поле Пароль скрыто под звездочками</t>
+  </si>
+  <si>
+    <t>Локализация</t>
+  </si>
+  <si>
+    <t>Текст отображается Кириллицей</t>
+  </si>
+  <si>
+    <t>Календарь отображается с понедельника по воскресенье</t>
+  </si>
+  <si>
+    <t>Удобство</t>
+  </si>
+  <si>
+    <t>Кнопки меню ведут на соответствующие разделы</t>
+  </si>
+  <si>
+    <t>Элементы выровнены и отображаются корректно</t>
+  </si>
+  <si>
+    <t>Возврат на предыдущий экран осуществляется</t>
+  </si>
+  <si>
+    <t>Подсказки в форме авторизации присутствуют</t>
+  </si>
+  <si>
+    <t>Установка</t>
+  </si>
+  <si>
+    <t>Приложение устанавливается</t>
+  </si>
+  <si>
+    <t>Приложение удаляется</t>
+  </si>
+  <si>
+    <t>Прерывания</t>
+  </si>
+  <si>
+    <t>Приложение сворачивается и разворачивается не изменяя состояния</t>
+  </si>
+  <si>
+    <t>Приложение не меняет состояния при разрыве соединения с интернетом</t>
+  </si>
+  <si>
+    <t>Приложение не меняет состояния при повороте экрана</t>
+  </si>
+  <si>
+    <t>Приложение работает при низком зарде батареи</t>
+  </si>
+  <si>
+    <t>Приложение работает при подключении хзарядного устройства</t>
+  </si>
+  <si>
+    <t>Входящее СМС не влияет на работу приложения</t>
+  </si>
+  <si>
+    <t>Входящий звонок не влияет на работу приложения</t>
+  </si>
+  <si>
+    <t>Подключения</t>
+  </si>
+  <si>
+    <t>Приложение работает через WIFI</t>
+  </si>
+  <si>
+    <t>Приложение работает через LTE</t>
+  </si>
+  <si>
+    <t>Работа приложения не изеняется при переключении с WIFI на мобильную сеть</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,6 +359,15 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -284,7 +395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -559,11 +670,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -610,18 +786,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -744,6 +908,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1039,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69:A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1054,824 +1278,1172 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.6" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="60" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="54" t="s">
+    <row r="2" spans="1:4" ht="27.6" customHeight="1">
+      <c r="A2" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="54"/>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="50"/>
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="54"/>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="50"/>
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="54"/>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="50"/>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="54"/>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="50"/>
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1">
-      <c r="A7" s="55"/>
-      <c r="B7" s="26" t="s">
+      <c r="C7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1">
+      <c r="A8" s="51"/>
+      <c r="B8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="26.4">
-      <c r="A8" s="51" t="s">
+      <c r="C8" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26.4">
+      <c r="A9" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="26.4">
-      <c r="A9" s="52"/>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.4">
+      <c r="A10" s="48"/>
+      <c r="B10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="52"/>
-      <c r="B10" s="11" t="s">
+      <c r="C10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="48"/>
+      <c r="B11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26.4">
-      <c r="A11" s="52"/>
-      <c r="B11" s="11" t="s">
+      <c r="C11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26.4">
+      <c r="A12" s="48"/>
+      <c r="B12" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="27" thickBot="1">
-      <c r="A12" s="53"/>
-      <c r="B12" s="32" t="s">
+      <c r="C12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="27" thickBot="1">
+      <c r="A13" s="49"/>
+      <c r="B13" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="56" t="s">
+      <c r="C13" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B14" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="26.4">
-      <c r="A14" s="54"/>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="26.4">
+      <c r="A15" s="50"/>
+      <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="26.4">
-      <c r="A15" s="54"/>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.4">
+      <c r="A16" s="50"/>
+      <c r="B16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="54"/>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="50"/>
+      <c r="B17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="27" thickBot="1">
-      <c r="A17" s="55"/>
-      <c r="B17" s="26" t="s">
+      <c r="D17" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="27" thickBot="1">
+      <c r="A18" s="51"/>
+      <c r="B18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C18" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="57" t="s">
+      <c r="D18" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B19" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C19" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="39" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="26.4">
-      <c r="A19" s="49"/>
-      <c r="B19" s="11" t="s">
+      <c r="D19" s="35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="26.4">
+      <c r="A20" s="45"/>
+      <c r="B20" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="26.4">
-      <c r="A20" s="49"/>
-      <c r="B20" s="11" t="s">
+      <c r="C20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="26.4">
+      <c r="A21" s="45"/>
+      <c r="B21" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D21" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="26.4">
-      <c r="A21" s="49"/>
-      <c r="B21" s="5" t="s">
+    <row r="22" spans="1:4" ht="26.4">
+      <c r="A22" s="45"/>
+      <c r="B22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="26.4">
-      <c r="A22" s="49"/>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="26.4">
+      <c r="A23" s="45"/>
+      <c r="B23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="27" thickBot="1">
-      <c r="A23" s="50"/>
-      <c r="B23" s="23" t="s">
+      <c r="C23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="27" thickBot="1">
+      <c r="A24" s="46"/>
+      <c r="B24" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="58" t="s">
+      <c r="C24" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B25" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="59"/>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="55"/>
+      <c r="B26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="59"/>
-      <c r="B26" s="14" t="s">
+      <c r="C26" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="55"/>
+      <c r="B27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="59"/>
-      <c r="B27" s="14" t="s">
+      <c r="C27" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="55"/>
+      <c r="B28" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="59"/>
-      <c r="B28" s="14" t="s">
+      <c r="C28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="55"/>
+      <c r="B29" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="59"/>
-      <c r="B29" s="14" t="s">
+      <c r="C29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="55"/>
+      <c r="B30" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="59"/>
-      <c r="B30" s="14" t="s">
+      <c r="C30" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="55"/>
+      <c r="B31" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="59"/>
-      <c r="B31" s="14" t="s">
+      <c r="C31" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="55"/>
+      <c r="B32" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="59"/>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="55"/>
+      <c r="B33" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="59"/>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="55"/>
+      <c r="B34" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1">
-      <c r="A34" s="60"/>
-      <c r="B34" s="41" t="s">
+      <c r="C34" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" thickBot="1">
+      <c r="A35" s="56"/>
+      <c r="B35" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="D34" s="28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="26.4">
-      <c r="A35" s="57" t="s">
+      <c r="C35" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="26.4">
+      <c r="A36" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B36" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" s="39" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="26.4">
-      <c r="A36" s="49"/>
-      <c r="B36" s="5" t="s">
+      <c r="C36" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="26.4">
+      <c r="A37" s="45"/>
+      <c r="B37" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="49"/>
-      <c r="B37" s="11" t="s">
+      <c r="C37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="45"/>
+      <c r="B38" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="49"/>
-      <c r="B38" s="11" t="s">
+      <c r="C38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="45"/>
+      <c r="B39" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="49"/>
-      <c r="B39" s="15" t="s">
+      <c r="C39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="45"/>
+      <c r="B40" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="49"/>
-      <c r="B40" s="15" t="s">
+      <c r="C40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="45"/>
+      <c r="B41" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D40" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="49"/>
-      <c r="B41" s="15" t="s">
+      <c r="C41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="45"/>
+      <c r="B42" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="49"/>
-      <c r="B42" s="15" t="s">
+      <c r="C42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="45"/>
+      <c r="B43" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="49"/>
-      <c r="B43" s="15" t="s">
+      <c r="C43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="45"/>
+      <c r="B44" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D43" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="49"/>
-      <c r="B44" s="15" t="s">
+      <c r="C44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="45"/>
+      <c r="B45" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D44" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="49"/>
-      <c r="B45" s="11" t="s">
+      <c r="C45" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="45"/>
+      <c r="B46" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="49"/>
-      <c r="B46" s="11" t="s">
+      <c r="C46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="45"/>
+      <c r="B47" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="49"/>
-      <c r="B47" s="15" t="s">
+      <c r="C47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="45"/>
+      <c r="B48" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="49"/>
-      <c r="B48" s="5" t="s">
+      <c r="C48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="45"/>
+      <c r="B49" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="26.4">
-      <c r="A49" s="49"/>
-      <c r="B49" s="5" t="s">
+      <c r="C49" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="26.4">
+      <c r="A50" s="45"/>
+      <c r="B50" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="26.4">
-      <c r="A50" s="49"/>
-      <c r="B50" s="5" t="s">
+      <c r="C50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="26.4">
+      <c r="A51" s="45"/>
+      <c r="B51" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="49"/>
-      <c r="B51" s="5" t="s">
+      <c r="C51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="45"/>
+      <c r="B52" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C52" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="26.4">
-      <c r="A52" s="49"/>
-      <c r="B52" s="5" t="s">
+      <c r="D52" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="26.4">
+      <c r="A53" s="45"/>
+      <c r="B53" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D52" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="49"/>
-      <c r="B53" s="5" t="s">
+      <c r="C53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="45"/>
+      <c r="B54" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D53" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="49"/>
-      <c r="B54" s="5" t="s">
+      <c r="C54" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="45"/>
+      <c r="B55" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D54" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="49"/>
-      <c r="B55" s="5" t="s">
+      <c r="C55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="45"/>
+      <c r="B56" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D55" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="49"/>
-      <c r="B56" s="5" t="s">
+      <c r="C56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="45"/>
+      <c r="B57" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D56" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="49"/>
-      <c r="B57" s="5" t="s">
+      <c r="C57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="45"/>
+      <c r="B58" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="49"/>
-      <c r="B58" s="5" t="s">
+      <c r="C58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="45"/>
+      <c r="B59" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="26.4">
-      <c r="A59" s="49"/>
-      <c r="B59" s="5" t="s">
+      <c r="C59" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="26.4">
+      <c r="A60" s="45"/>
+      <c r="B60" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D59" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="15" thickBot="1">
-      <c r="A60" s="50"/>
-      <c r="B60" s="23" t="s">
+      <c r="C60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" thickBot="1">
+      <c r="A61" s="46"/>
+      <c r="B61" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="D60" s="25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="15" thickBot="1">
-      <c r="A61" s="44" t="s">
+      <c r="C61" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15" thickBot="1">
+      <c r="A62" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B61" s="45" t="s">
+      <c r="B62" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C61" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="D61" s="47" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="48" t="s">
+      <c r="C62" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B62" s="40" t="s">
+      <c r="B63" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C63" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D62" s="35" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="49"/>
-      <c r="B63" s="5" t="s">
+      <c r="D63" s="31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="45"/>
+      <c r="B64" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D63" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="49"/>
-      <c r="B64" s="8" t="s">
+      <c r="C64" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="45"/>
+      <c r="B65" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D64" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="26.4">
-      <c r="A65" s="49"/>
-      <c r="B65" s="5" t="s">
+      <c r="C65" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="26.4">
+      <c r="A66" s="45"/>
+      <c r="B66" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D65" s="22" t="s">
+      <c r="C66" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="27" thickBot="1">
-      <c r="A66" s="50"/>
-      <c r="B66" s="23" t="s">
+    <row r="67" spans="1:4" ht="27" thickBot="1">
+      <c r="A67" s="63"/>
+      <c r="B67" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="C66" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="D66" s="25" t="s">
+      <c r="C67" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" s="66" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="68" spans="1:4" ht="31.8" customHeight="1">
+      <c r="A68" s="67" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" s="68"/>
+      <c r="C68" s="68"/>
+      <c r="D68" s="69"/>
+    </row>
+    <row r="69" spans="1:4" ht="28.8">
+      <c r="A69" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="28.8">
+      <c r="A70" s="70"/>
+      <c r="B70" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="70"/>
+      <c r="B71" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="70"/>
+      <c r="B72" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="28.8">
+      <c r="A73" s="70"/>
+      <c r="B73" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="28.8">
+      <c r="A74" s="70"/>
+      <c r="B74" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="28.8">
+      <c r="A75" s="70"/>
+      <c r="B75" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="70"/>
+      <c r="B76" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="71" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="28.8">
+      <c r="A78" s="71"/>
+      <c r="B78" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="70" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D79" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="70"/>
+      <c r="B80" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="70"/>
+      <c r="B81" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="70"/>
+      <c r="B82" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="73"/>
+      <c r="B84" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D84" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="28.8">
+      <c r="A85" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="28.8">
+      <c r="A86" s="70"/>
+      <c r="B86" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D86" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="28.8">
+      <c r="A87" s="70"/>
+      <c r="B87" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D87" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="74"/>
+      <c r="B88" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D88" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="28.8">
+      <c r="A89" s="74"/>
+      <c r="B89" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D89" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="74"/>
+      <c r="B90" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D90" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="74"/>
+      <c r="B91" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D91" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="75"/>
+      <c r="B93" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D93" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="29.4" thickBot="1">
+      <c r="A94" s="76"/>
+      <c r="B94" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="C94" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D94" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="A35:A60"/>
-    <mergeCell ref="A24:A34"/>
+  <mergeCells count="15">
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A85:A91"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A69:A76"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="A63:A67"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A36:A61"/>
+    <mergeCell ref="A25:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>